<commit_message>
Criando E-mail para os Gerentes
</commit_message>
<xml_diff>
--- a/Bases de Dados/Emails.xlsx
+++ b/Bases de Dados/Emails.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Google Drive\Python Impressionador\Projeto_AutomacaoIndicadores\Bases de Dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bulllasa-my.sharepoint.com/personal/gabriel_souza_bullla_com_br/Documents/ws-projetos-python-impressionador/automacao-processo-indicadores/Bases de Dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3856DD-4A41-42A6-8CEE-9B800498E7C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{FF3856DD-4A41-42A6-8CEE-9B800498E7C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39254199-7ADC-4AC8-B9CA-8F1DA227FC0D}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{EE9D8D8A-F7B1-481B-B9DF-10FF6CFE8B3E}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{EE9D8D8A-F7B1-481B-B9DF-10FF6CFE8B3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -180,63 +180,6 @@
     <t>Diretoria</t>
   </si>
   <si>
-    <t>pythonimpressionador+helena@gmail.com</t>
-  </si>
-  <si>
-    <t>pythonimpressionador+alice@gmail.com</t>
-  </si>
-  <si>
-    <t>pythonimpressionador+laura@gmail.com</t>
-  </si>
-  <si>
-    <t>pythonimpressionador+manuela@gmail.com</t>
-  </si>
-  <si>
-    <t>pythonimpressionador+valentina@gmail.com</t>
-  </si>
-  <si>
-    <t>pythonimpressionador+sophia@gmail.com</t>
-  </si>
-  <si>
-    <t>pythonimpressionador+isabella@gmail.com</t>
-  </si>
-  <si>
-    <t>pythonimpressionador+luiza@gmail.com</t>
-  </si>
-  <si>
-    <t>pythonimpressionador+lorena@gmail.com</t>
-  </si>
-  <si>
-    <t>pythonimpressionador+miguel@gmail.com</t>
-  </si>
-  <si>
-    <t>pythonimpressionador+arthur@gmail.com</t>
-  </si>
-  <si>
-    <t>pythonimpressionador+heitor@gmail.com</t>
-  </si>
-  <si>
-    <t>pythonimpressionador+bernardo@gmail.com</t>
-  </si>
-  <si>
-    <t>pythonimpressionador+davi@gmail.com</t>
-  </si>
-  <si>
-    <t>pythonimpressionador+lorenzo@gmail.com</t>
-  </si>
-  <si>
-    <t>pythonimpressionador+gabriel@gmail.com</t>
-  </si>
-  <si>
-    <t>pythonimpressionador+pedro@gmail.com</t>
-  </si>
-  <si>
-    <t>pythonimpressionador+benjamin@gmail.com</t>
-  </si>
-  <si>
-    <t>pythonimpressionador+diretoria@gmail.com</t>
-  </si>
-  <si>
     <t>Heloisa</t>
   </si>
   <si>
@@ -255,32 +198,89 @@
     <t>Theo</t>
   </si>
   <si>
-    <t>pythonimpressionador+heloisa@gmail.com</t>
-  </si>
-  <si>
-    <t>pythonimpressionador+julia@gmail.com</t>
-  </si>
-  <si>
-    <t>pythonimpressionador+livia@gmail.com</t>
-  </si>
-  <si>
-    <t>pythonimpressionador+cecilia@gmail.com</t>
-  </si>
-  <si>
-    <t>pythonimpressionador+eloa@gmail.com</t>
-  </si>
-  <si>
-    <t>pythonimpressionador+theo@gmail.com</t>
-  </si>
-  <si>
-    <t>pythonimpressionador+maria_luiza@gmail.com</t>
+    <t>gsoaresdesouzaaws+helena@gmail.com</t>
+  </si>
+  <si>
+    <t>gsoaresdesouzaaws+alice@gmail.com</t>
+  </si>
+  <si>
+    <t>gsoaresdesouzaaws+laura@gmail.com</t>
+  </si>
+  <si>
+    <t>gsoaresdesouzaaws+manuela@gmail.com</t>
+  </si>
+  <si>
+    <t>gsoaresdesouzaaws+valentina@gmail.com</t>
+  </si>
+  <si>
+    <t>gsoaresdesouzaaws+sophia@gmail.com</t>
+  </si>
+  <si>
+    <t>gsoaresdesouzaaws+isabella@gmail.com</t>
+  </si>
+  <si>
+    <t>gsoaresdesouzaaws+heloisa@gmail.com</t>
+  </si>
+  <si>
+    <t>gsoaresdesouzaaws+luiza@gmail.com</t>
+  </si>
+  <si>
+    <t>gsoaresdesouzaaws+julia@gmail.com</t>
+  </si>
+  <si>
+    <t>gsoaresdesouzaaws+lorena@gmail.com</t>
+  </si>
+  <si>
+    <t>gsoaresdesouzaaws+livia@gmail.com</t>
+  </si>
+  <si>
+    <t>gsoaresdesouzaaws+maria_luiza@gmail.com</t>
+  </si>
+  <si>
+    <t>gsoaresdesouzaaws+cecilia@gmail.com</t>
+  </si>
+  <si>
+    <t>gsoaresdesouzaaws+eloa@gmail.com</t>
+  </si>
+  <si>
+    <t>gsoaresdesouzaaws+miguel@gmail.com</t>
+  </si>
+  <si>
+    <t>gsoaresdesouzaaws+arthur@gmail.com</t>
+  </si>
+  <si>
+    <t>gsoaresdesouzaaws+heitor@gmail.com</t>
+  </si>
+  <si>
+    <t>gsoaresdesouzaaws+bernardo@gmail.com</t>
+  </si>
+  <si>
+    <t>gsoaresdesouzaaws+davi@gmail.com</t>
+  </si>
+  <si>
+    <t>gsoaresdesouzaaws+theo@gmail.com</t>
+  </si>
+  <si>
+    <t>gsoaresdesouzaaws+lorenzo@gmail.com</t>
+  </si>
+  <si>
+    <t>gsoaresdesouzaaws+gabriel@gmail.com</t>
+  </si>
+  <si>
+    <t>gsoaresdesouzaaws+pedro@gmail.com</t>
+  </si>
+  <si>
+    <t>gsoaresdesouzaaws+benjamin@gmail.com</t>
+  </si>
+  <si>
+    <t>gsoaresdesouzaaws+diretoria@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,6 +292,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -318,9 +326,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -636,19 +645,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D81E77-7AEF-4DB7-8688-DEDDD091CFFB}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.62890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.3671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -659,7 +668,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -667,11 +676,11 @@
         <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -679,11 +688,11 @@
         <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -691,10 +700,10 @@
         <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -702,10 +711,10 @@
         <v>34</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -713,10 +722,10 @@
         <v>36</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -724,10 +733,10 @@
         <v>38</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -735,21 +744,21 @@
         <v>39</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -757,21 +766,21 @@
         <v>42</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -779,21 +788,21 @@
         <v>45</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -801,32 +810,32 @@
         <v>46</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -834,10 +843,10 @@
         <v>29</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -845,10 +854,10 @@
         <v>31</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -856,10 +865,10 @@
         <v>33</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -867,10 +876,10 @@
         <v>35</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -878,21 +887,21 @@
         <v>37</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -900,10 +909,11 @@
         <v>40</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>75</v>
+      </c>
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -911,10 +921,10 @@
         <v>41</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -922,10 +932,10 @@
         <v>43</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -933,10 +943,10 @@
         <v>44</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -944,38 +954,11 @@
         <v>47</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{71E13B65-9239-473E-B00B-24152BE46E62}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{E3106FEB-106F-4653-B503-E2D2031143F8}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{B6EBA633-9A57-4B4B-96B4-C65CFAD1BB3E}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{7823E53E-AF09-484D-A82D-90E56D3B173C}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{3741F77C-FA16-4C22-B015-4FDF829B5647}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{E0868D17-25A2-487B-AA15-484F6B02EBA7}"/>
-    <hyperlink ref="C8" r:id="rId7" xr:uid="{B6F8659F-A0CB-412D-AE6A-9DA852BFAA32}"/>
-    <hyperlink ref="C9" r:id="rId8" xr:uid="{4CFCBEB2-A644-4E59-9788-1DDF09FAF464}"/>
-    <hyperlink ref="C10" r:id="rId9" xr:uid="{38F81A3D-BB76-4DBF-B55C-183FC4B858A7}"/>
-    <hyperlink ref="C11" r:id="rId10" xr:uid="{98973E91-31EC-40FD-86B0-ED8A4168C6E8}"/>
-    <hyperlink ref="C12" r:id="rId11" xr:uid="{03A322C5-0A08-4680-8550-E77955A4AE16}"/>
-    <hyperlink ref="C13" r:id="rId12" xr:uid="{E5CB0419-824E-4DB2-A37A-D3C4C77E1115}"/>
-    <hyperlink ref="C15" r:id="rId13" xr:uid="{59E0BF81-A494-4E83-8798-A91BEBA8D604}"/>
-    <hyperlink ref="C16" r:id="rId14" xr:uid="{ACE724F6-B50F-4C54-BEB0-05F796CEB518}"/>
-    <hyperlink ref="C17" r:id="rId15" xr:uid="{97ADDF58-A02A-4AB6-92C6-A696B385AA7C}"/>
-    <hyperlink ref="C18" r:id="rId16" xr:uid="{468AA824-B854-4C50-AE64-62AB564D2BC8}"/>
-    <hyperlink ref="C19" r:id="rId17" xr:uid="{D68730A0-9B08-47EA-B08B-D9AF34A604C6}"/>
-    <hyperlink ref="C20" r:id="rId18" xr:uid="{DC9B9350-B3A1-42F7-AC7F-FA19215DAC1C}"/>
-    <hyperlink ref="C21" r:id="rId19" xr:uid="{2B72A44B-E3AB-4DC9-843D-E086A5935BBD}"/>
-    <hyperlink ref="C22" r:id="rId20" xr:uid="{86DE27C8-7A8B-4539-BDDF-78A25128E590}"/>
-    <hyperlink ref="C23" r:id="rId21" xr:uid="{DA1C7256-28A5-4CC6-B93E-1D00A4600C54}"/>
-    <hyperlink ref="C24" r:id="rId22" xr:uid="{4218CF6B-06BF-4E28-B5ED-DB65662FB86F}"/>
-    <hyperlink ref="C25" r:id="rId23" xr:uid="{AFD4FC21-C827-47BB-A10B-8F182A528B87}"/>
-    <hyperlink ref="C26" r:id="rId24" xr:uid="{A077F048-53D0-4C90-9D38-4531C608CEEB}"/>
-    <hyperlink ref="C27" r:id="rId25" xr:uid="{9146DF61-FD66-4AC6-8767-2D00EC98E736}"/>
-    <hyperlink ref="C14" r:id="rId26" xr:uid="{5FFD0C79-EDBB-417E-98DA-5E77D27BBC40}"/>
-  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>